<commit_message>
all kinds of revise before submit
</commit_message>
<xml_diff>
--- a/课程设计/单周期硬布线控制器表达式自动生成(2019-10-29).xlsx
+++ b/课程设计/单周期硬布线控制器表达式自动生成(2019-10-29).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ComputerOrganization\课程设计\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD14439B-A710-48BF-B216-63789AF5E149}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1709B691-5EA1-42D5-9C6E-D355B4A6479E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="129">
   <si>
     <t>#</t>
   </si>
@@ -891,10 +891,6 @@
   </si>
   <si>
     <t xml:space="preserve">   </t>
-    <phoneticPr fontId="28" type="noConversion"/>
-  </si>
-  <si>
-    <t>ch</t>
     <phoneticPr fontId="28" type="noConversion"/>
   </si>
 </sst>
@@ -2187,7 +2183,7 @@
   <dimension ref="A1:AO65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AT17" sqref="AT17"/>
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
@@ -4152,8 +4148,8 @@
       <c r="AN18" s="24"/>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.4">
-      <c r="A19" s="27" t="s">
-        <v>129</v>
+      <c r="A19" s="27">
+        <v>18</v>
       </c>
       <c r="B19" s="27" t="s">
         <v>48</v>

</xml_diff>